<commit_message>
Fixed error in normalize. Cleaned up code.
</commit_message>
<xml_diff>
--- a/conversions.xlsx
+++ b/conversions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\source\repos\Recipe volume to weight\Recipe volume to weight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\source\repos\Recipe-volume-to-weight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8FE5DD-5E17-48C9-BA14-B39ED342BED7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D382DE1B-CD0E-4FF3-8215-D67B25BDAEB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="-90" windowWidth="18430" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="356">
   <si>
     <t>almonds, ground</t>
   </si>
@@ -1085,10 +1085,22 @@
     <t>confectioner sugar</t>
   </si>
   <si>
-    <t>Normal ingredient name</t>
-  </si>
-  <si>
-    <t>Equivalent ingredient names</t>
+    <t>packed brown sugar</t>
+  </si>
+  <si>
+    <t>brown sugar, packed</t>
+  </si>
+  <si>
+    <t>Equivalent names</t>
+  </si>
+  <si>
+    <t>Normal name</t>
+  </si>
+  <si>
+    <t>powder sugar</t>
+  </si>
+  <si>
+    <t>icing sugar</t>
   </si>
 </sst>
 </file>
@@ -1287,11 +1299,11 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1822,10 +1834,10 @@
   </sheetPr>
   <dimension ref="A1:AD304"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="P4" sqref="P4"/>
+      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18685,8 +18697,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId6" name="CommandButton">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId7">
+        <control shapeId="1032" r:id="rId6" name="TempCombo">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>41275</xdr:colOff>
+                <xdr:row>0</xdr:row>
+                <xdr:rowOff>41275</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>596900</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>101600</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId6" name="TempCombo"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1046" r:id="rId8" name="CommandButton">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -18705,32 +18742,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1046" r:id="rId6" name="CommandButton"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId8" name="TempCombo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>41275</xdr:colOff>
-                <xdr:row>0</xdr:row>
-                <xdr:rowOff>41275</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>596900</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>101600</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId8" name="TempCombo"/>
+        <control shapeId="1046" r:id="rId8" name="CommandButton"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18739,10 +18751,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C456A2-2442-4B14-A5A2-002CEFEDB788}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18750,29 +18762,29 @@
     <col min="1" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="30" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D1" s="30" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.75">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A2" s="29" t="s">
         <v>328</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="F2" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="G2" s="29" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A3" s="29" t="s">
         <v>331</v>
       </c>
@@ -18783,7 +18795,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A4" s="29" t="s">
         <v>334</v>
       </c>
@@ -18794,7 +18806,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A5" s="29" t="s">
         <v>336</v>
       </c>
@@ -18802,7 +18814,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A6" s="29" t="s">
         <v>210</v>
       </c>
@@ -18819,18 +18831,18 @@
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A7" s="29" t="s">
-        <v>342</v>
+        <v>209</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>341</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.75">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A8" s="29" t="s">
         <v>142</v>
       </c>
@@ -18843,16 +18855,28 @@
       <c r="H8" s="29" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="J8" s="29" t="s">
+        <v>350</v>
+      </c>
+      <c r="L8" s="29" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A9" s="29" t="s">
         <v>146</v>
       </c>
       <c r="D9" s="29" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.75">
+      <c r="F9" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A10" s="29" t="s">
         <v>144</v>
       </c>

</xml_diff>

<commit_message>
Changed scraper to seperate class. Added websites to scraper.
</commit_message>
<xml_diff>
--- a/conversions.xlsx
+++ b/conversions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\source\repos\Recipe-volume-to-weight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D382DE1B-CD0E-4FF3-8215-D67B25BDAEB7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581E4697-962D-4697-934F-3801A25C1A1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="-90" windowWidth="18430" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="357">
   <si>
     <t>almonds, ground</t>
   </si>
@@ -1101,6 +1101,9 @@
   </si>
   <si>
     <t>icing sugar</t>
+  </si>
+  <si>
+    <t>powdered sugar same as icing sugar or confectioners sugar</t>
   </si>
 </sst>
 </file>
@@ -1299,11 +1302,11 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D30-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18697,8 +18700,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId6" name="TempCombo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="1046" r:id="rId6" name="CommandButton">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>3175</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>44450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId6" name="CommandButton"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId8" name="TempCombo">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18717,32 +18745,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1032" r:id="rId6" name="TempCombo"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId8" name="CommandButton">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>3175</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>44450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId8" name="CommandButton"/>
+        <control shapeId="1032" r:id="rId8" name="TempCombo"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18754,7 +18757,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18875,6 +18878,9 @@
       <c r="H9" s="29" t="s">
         <v>355</v>
       </c>
+      <c r="J9" s="29" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.75">
       <c r="A10" s="29" t="s">

</xml_diff>

<commit_message>
Added sites to scraper, selection option, and static method convert_print.
</commit_message>
<xml_diff>
--- a/conversions.xlsx
+++ b/conversions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bilal\source\repos\Recipe-volume-to-weight\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581E4697-962D-4697-934F-3801A25C1A1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EA63823-3C1F-4998-A058-574EBFDF1656}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="-90" windowWidth="18430" windowHeight="10980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="366">
   <si>
     <t>almonds, ground</t>
   </si>
@@ -1104,6 +1104,33 @@
   </si>
   <si>
     <t>powdered sugar same as icing sugar or confectioners sugar</t>
+  </si>
+  <si>
+    <t>don't convert</t>
+  </si>
+  <si>
+    <t>cornstarch</t>
+  </si>
+  <si>
+    <t>cornflour</t>
+  </si>
+  <si>
+    <t>corn starch</t>
+  </si>
+  <si>
+    <t>corn flour</t>
+  </si>
+  <si>
+    <t>dark corn syrup</t>
+  </si>
+  <si>
+    <t>light corn syrup</t>
+  </si>
+  <si>
+    <t>strawberries</t>
+  </si>
+  <si>
+    <t>fresh strawberries</t>
   </si>
 </sst>
 </file>
@@ -1837,10 +1864,10 @@
   </sheetPr>
   <dimension ref="A1:AD304"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="M1" zoomScale="80" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="P237" sqref="P237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18754,10 +18781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C456A2-2442-4B14-A5A2-002CEFEDB788}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -18765,135 +18792,187 @@
     <col min="1" max="16384" width="8.7265625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="30" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" s="30" customFormat="1" x14ac:dyDescent="0.75">
       <c r="A1" s="30" t="s">
         <v>353</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="C1" s="30" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="C2" s="29" t="s">
         <v>327</v>
       </c>
+      <c r="E2" s="29" t="s">
+        <v>329</v>
+      </c>
       <c r="F2" s="29" t="s">
-        <v>329</v>
-      </c>
-      <c r="G2" s="29" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A3" s="29" t="s">
         <v>331</v>
       </c>
+      <c r="C3" s="29" t="s">
+        <v>332</v>
+      </c>
       <c r="D3" s="29" t="s">
-        <v>332</v>
-      </c>
-      <c r="E3" s="29" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A4" s="29" t="s">
         <v>334</v>
       </c>
+      <c r="C4" s="29" t="s">
+        <v>335</v>
+      </c>
       <c r="D4" s="29" t="s">
-        <v>335</v>
-      </c>
-      <c r="E4" s="29" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A5" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="29" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A6" s="29" t="s">
         <v>210</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="C6" s="29" t="s">
         <v>337</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="E6" s="29" t="s">
         <v>338</v>
       </c>
+      <c r="G6" s="29" t="s">
+        <v>339</v>
+      </c>
       <c r="H6" s="29" t="s">
-        <v>339</v>
-      </c>
-      <c r="I6" s="29" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A7" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="C7" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="E7" s="29" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A8" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="C8" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="E8" s="29" t="s">
         <v>344</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="G8" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="I8" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="K8" s="29" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A9" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="C9" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="E9" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="H9" s="29" t="s">
+      <c r="G9" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="J9" s="29" t="s">
+      <c r="I9" s="29" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A10" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="C10" s="29" t="s">
         <v>346</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="E10" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="H10" s="29" t="s">
+      <c r="G10" s="29" t="s">
         <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A11" s="29" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>358</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>359</v>
+      </c>
+      <c r="F12" s="29" t="s">
+        <v>360</v>
+      </c>
+      <c r="H12" s="29" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>284</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A14" t="s">
+        <v>285</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+      <c r="A15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>